<commit_message>
update result 20201130 & update plan 20201201
</commit_message>
<xml_diff>
--- a/20201130.xlsx
+++ b/20201130.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1193DF9-98C7-498A-B429-B87A1964568B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654E6FE3-F7AF-47DF-99D0-39ADA116BA3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>일</t>
   </si>
@@ -190,10 +190,6 @@
   </si>
   <si>
     <t>체크사항</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. NCT세트 피앤이로부터 전달 받으면 사설IP, 외부IP에 따라 타임아웃 적용이 다르게 되던 현상 테스트 할 것</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
@@ -209,10 +205,6 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>저번주에 못지킨 월수금 약속 지키기</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>어둠 코딩 (노트북 들고가서 와이어샤크로 패킷 캡쳐하기)</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
@@ -234,6 +226,37 @@
   </si>
   <si>
     <t>모빌리티 보드 수정</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. F7
+ - 로그 분할
+  -&gt; 패킷로그와 시스템로그를 분할 (완)
+  -&gt; 로그를 하루단위로 변경 (로그 제목은 ex)201130.csv등으로 변경) (완)
+   =&gt; 에이징 테스트 진행할 것
+  -&gt; 로그제목을 xxxxxx-00으로 변경 및 100MB넘을 시 분할 (진행중)
+2. 모빌리티
+ - MAC구매 건은 추후 결정 (일단 대충사용)
+ - 5ea전달 (피앤이, 20201127버젼, 보드수정, MAC 85~89)</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>저번주에 못지킨 월수금 약속 지키기(운동, 금식, 술안먹기, 아침에 공부)
+33.3%</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. NCT세트 피앤이로부터 전달 받으면 사설IP, 외부IP에 따라 타임아웃 적용이 다르게 되던 현상 테스트 할 것
+2. 로그 이름이 날짜 변경 시 변경되는지 에이징 테스트 할 것</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>비타민 까먹음</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>젤힘든구간… 늦잠
+1시30분에 잠들어야 지킬 수 있음..</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -407,7 +430,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -615,6 +638,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -921,7 +968,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -937,74 +984,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="1" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1538,8 +1600,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1580,7 +1642,7 @@
         <v>21</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" t="s">
@@ -1600,23 +1662,29 @@
       </c>
     </row>
     <row r="3" spans="2:15" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="22" t="s">
+      <c r="D3" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19" t="s">
-        <v>48</v>
+      <c r="H3" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" t="s">
@@ -1630,14 +1698,14 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="6"/>
       <c r="J4" s="4"/>
       <c r="K4" t="s">
         <v>11</v>
@@ -1647,14 +1715,14 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="6"/>
       <c r="J5" s="4"/>
       <c r="K5" t="s">
         <v>12</v>
@@ -1664,14 +1732,14 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="6"/>
       <c r="J6" s="4"/>
       <c r="K6" t="s">
         <v>10</v>
@@ -1681,14 +1749,14 @@
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="6"/>
       <c r="J7" s="4"/>
       <c r="K7" t="s">
         <v>8</v>
@@ -1702,14 +1770,14 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="6"/>
       <c r="J8" s="4"/>
       <c r="K8" t="s">
         <v>4</v>
@@ -1719,228 +1787,228 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="6"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="6"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="2:15" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="2:15" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="14" t="s">
+      <c r="D15" s="21"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="2:15" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="2:10" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="14" t="s">
+      <c r="D17" s="21"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="2:15" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="2:10" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="6"/>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="2:10" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="6"/>
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="6"/>
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="6"/>
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="6"/>
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
+      <c r="C23" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="26"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="7"/>
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
@@ -1948,14 +2016,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="H3:H23"/>
+    <mergeCell ref="E3:E23"/>
+    <mergeCell ref="I3:I23"/>
     <mergeCell ref="F3:F23"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
-    <mergeCell ref="D3:D8"/>
     <mergeCell ref="G3:G23"/>
-    <mergeCell ref="H3:H23"/>
-    <mergeCell ref="E3:E23"/>
-    <mergeCell ref="I3:I23"/>
+    <mergeCell ref="D3:D9"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>